<commit_message>
added venv, updated the log in designs, moved output and inpus css to static folder
</commit_message>
<xml_diff>
--- a/aspirematch/database/uploads/xl.xlsx
+++ b/aspirematch/database/uploads/xl.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\f4\aspirematch\database\uploads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elvie\HertzKinLetigio\aspirematch\database\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEEEB0A9-CA51-43BF-913A-2CAD596A36F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90E504A0-2197-4BDE-9AE5-14FD63E2B7EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" xr2:uid="{29E38EED-B63D-43BF-87E0-B342A6A7E61D}"/>
+    <workbookView xWindow="3030" yWindow="1245" windowWidth="15375" windowHeight="7875" xr2:uid="{29E38EED-B63D-43BF-87E0-B342A6A7E61D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Hertz</t>
   </si>
@@ -76,6 +76,18 @@
   </si>
   <si>
     <t>l@gmail.com</t>
+  </si>
+  <si>
+    <t>el</t>
+  </si>
+  <si>
+    <t>T.</t>
+  </si>
+  <si>
+    <t>Gil</t>
+  </si>
+  <si>
+    <t>e@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -438,22 +450,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F57B50A2-4D0C-4C37-AC93-B42802B65148}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="10.54296875" customWidth="1"/>
-    <col min="3" max="3" width="14.08984375" customWidth="1"/>
-    <col min="4" max="4" width="11.81640625" customWidth="1"/>
-    <col min="5" max="5" width="15.6328125" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -470,7 +482,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -487,7 +499,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -504,7 +516,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -519,6 +531,23 @@
       </c>
       <c r="E4" s="1" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -526,6 +555,7 @@
     <hyperlink ref="E2" r:id="rId1" xr:uid="{195FB06B-6819-4CD0-8FF6-5A046BFF6694}"/>
     <hyperlink ref="E3" r:id="rId2" xr:uid="{612417C1-4955-40F2-9B1C-4D5D4D58C886}"/>
     <hyperlink ref="E4" r:id="rId3" xr:uid="{C55B36A7-7E3F-41A4-854E-2B2B8DD6B339}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{93205B9A-0277-435A-B656-105BD21A0F3B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>